<commit_message>
[ADD] local coverage of unit tests for choerodon-liquibase comes 83%
</commit_message>
<xml_diff>
--- a/choerodon-liquibase/src/test/resources/script/db/2018-03-27-init-data.xlsx
+++ b/choerodon-liquibase/src/test/resources/script/db/2018-03-27-init-data.xlsx
@@ -2384,10 +2384,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="40">
     <font>
@@ -2496,6 +2496,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -2503,8 +2518,64 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2526,61 +2597,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2594,38 +2625,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2700,7 +2700,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2712,7 +2718,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2724,13 +2730,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2742,7 +2796,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2754,43 +2838,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2808,19 +2862,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2832,55 +2880,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3002,21 +3002,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -3041,11 +3026,37 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3067,17 +3078,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -3089,142 +3089,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="29" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3762,8 +3762,8 @@
   <sheetPr/>
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="B8" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="7"/>
@@ -4323,8 +4323,8 @@
   <sheetPr/>
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelRow="7" outlineLevelCol="7"/>

</xml_diff>

<commit_message>
[ADD] refactor unit tests for choerodon-liquibase
</commit_message>
<xml_diff>
--- a/choerodon-liquibase/src/test/resources/script/db/2018-03-27-init-data.xlsx
+++ b/choerodon-liquibase/src/test/resources/script/db/2018-03-27-init-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8925" tabRatio="987" activeTab="1"/>
+    <workbookView windowWidth="20385" windowHeight="8925" tabRatio="987" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -2384,10 +2384,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="40">
     <font>
@@ -2496,9 +2496,33 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2511,39 +2535,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2559,6 +2551,21 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -2567,37 +2574,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2618,7 +2595,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2626,6 +2603,29 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2700,13 +2700,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2718,13 +2712,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2736,13 +2730,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2754,91 +2748,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2856,7 +2766,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2874,13 +2880,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3026,6 +3026,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -3046,17 +3057,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3089,142 +3089,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="11" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="29" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3763,7 +3763,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView topLeftCell="B8" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="7"/>
@@ -4323,7 +4323,7 @@
   <sheetPr/>
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -4393,10 +4393,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="D7:I17"/>
+  <dimension ref="D7:I18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -4593,6 +4593,23 @@
         <v>62</v>
       </c>
       <c r="I17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="5:9">
+      <c r="E18" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" t="s">
+        <v>81</v>
+      </c>
+      <c r="G18" t="s">
+        <v>61</v>
+      </c>
+      <c r="H18" t="s">
+        <v>62</v>
+      </c>
+      <c r="I18" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[ADD] add unit tests for choerodon-liquibase
</commit_message>
<xml_diff>
--- a/choerodon-liquibase/src/test/resources/script/db/2018-03-27-init-data.xlsx
+++ b/choerodon-liquibase/src/test/resources/script/db/2018-03-27-init-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8925" tabRatio="987" activeTab="2"/>
+    <workbookView windowWidth="20385" windowHeight="8925" tabRatio="987" firstSheet="6" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -2376,7 +2376,7 @@
     <t>MAX_ERROR_TIME</t>
   </si>
   <si>
-    <t>LOCKED_EXPIRE_TIME</t>
+    <t>LOCKED_EXPIRE_TIME(BIGINT)</t>
   </si>
 </sst>
 </file>
@@ -2384,16 +2384,22 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="40">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="DengXian"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
@@ -2447,12 +2453,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
@@ -2495,6 +2495,45 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -2504,31 +2543,29 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2543,66 +2580,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2623,11 +2601,33 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2700,25 +2700,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2736,7 +2730,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2748,139 +2874,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2987,56 +2987,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -3062,6 +3012,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -3078,9 +3043,44 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3089,148 +3089,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="10" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="36" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3238,22 +3238,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3265,19 +3268,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="48" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="48" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="48" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="48" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3295,16 +3295,16 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3331,7 +3331,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3349,16 +3349,16 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3770,7 +3770,7 @@
   <cols>
     <col min="1" max="2" width="9.74814814814815" style="18"/>
     <col min="3" max="3" width="100.622222222222" customWidth="1"/>
-    <col min="4" max="4" width="9.74814814814815" style="6"/>
+    <col min="4" max="4" width="9.74814814814815" style="7"/>
     <col min="5" max="1025" width="9.74814814814815"/>
   </cols>
   <sheetData>
@@ -3936,7 +3936,7 @@
       <c r="E19" s="33"/>
     </row>
     <row r="20" ht="18" spans="3:4">
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="12" t="s">
         <v>31</v>
       </c>
       <c r="D20" s="34" t="s">
@@ -3944,7 +3944,7 @@
       </c>
     </row>
     <row r="21" ht="18" spans="3:4">
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="12" t="s">
         <v>33</v>
       </c>
       <c r="D21" s="34" t="s">
@@ -3952,7 +3952,7 @@
       </c>
     </row>
     <row r="22" ht="18" spans="3:4">
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="12" t="s">
         <v>35</v>
       </c>
       <c r="D22" s="23" t="s">
@@ -3960,7 +3960,7 @@
       </c>
     </row>
     <row r="23" ht="18" spans="3:4">
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D23" s="23" t="s">
@@ -4014,7 +4014,7 @@
   <sheetPr/>
   <dimension ref="D7:I8"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -4031,35 +4031,35 @@
       <c r="D7" t="s">
         <v>171</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="I7" s="1"/>
+      <c r="I7" s="2"/>
     </row>
     <row r="8" spans="4:9">
-      <c r="D8" s="1"/>
-      <c r="E8" s="1" t="s">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="I8" s="1"/>
+      <c r="I8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4085,65 +4085,65 @@
   </cols>
   <sheetData>
     <row r="7" spans="4:10">
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="J7" s="1"/>
+      <c r="J7" s="2"/>
     </row>
     <row r="8" spans="4:10">
-      <c r="D8" s="1"/>
-      <c r="E8" s="1" t="s">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="G8" s="1" t="str">
+      <c r="G8" s="2" t="str">
         <f>FD_LOOKUP!E8</f>
         <v>TIME_ZONE</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="J8" s="1"/>
+      <c r="J8" s="2"/>
     </row>
     <row r="9" spans="4:10">
-      <c r="D9" s="1"/>
-      <c r="E9" s="1" t="s">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="G9" s="1" t="str">
+      <c r="G9" s="2" t="str">
         <f>FD_LOOKUP!E8</f>
         <v>TIME_ZONE</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="J9" s="1"/>
+      <c r="J9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4224,13 +4224,13 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="D7:N8"/>
+  <dimension ref="D7:N9"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelRow="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
     <col min="4" max="4" width="22.7481481481481" customWidth="1"/>
     <col min="5" max="5" width="11.2518518518519" customWidth="1"/>
@@ -4275,7 +4275,7 @@
       <c r="M7" t="s">
         <v>195</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" s="1" t="s">
         <v>196</v>
       </c>
     </row>
@@ -4309,6 +4309,38 @@
       </c>
       <c r="N8">
         <v>600</v>
+      </c>
+    </row>
+    <row r="9" spans="5:14">
+      <c r="E9" t="s">
+        <v>186</v>
+      </c>
+      <c r="F9" t="s">
+        <v>186</v>
+      </c>
+      <c r="G9" t="s">
+        <v>186</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>3</v>
+      </c>
+      <c r="M9">
+        <v>5</v>
+      </c>
+      <c r="N9">
+        <v>600.12</v>
       </c>
     </row>
   </sheetData>
@@ -4337,16 +4369,16 @@
   </cols>
   <sheetData>
     <row r="1" ht="18" spans="1:4">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>46</v>
       </c>
     </row>
@@ -4354,31 +4386,31 @@
       <c r="D7" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="7" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="1" t="s">
         <v>52</v>
       </c>
       <c r="E8" s="17"/>
       <c r="F8" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="H8" s="6"/>
+      <c r="H8" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -4395,7 +4427,7 @@
   <sheetPr/>
   <dimension ref="D7:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
@@ -4645,31 +4677,31 @@
   </cols>
   <sheetData>
     <row r="1" ht="18" spans="1:5">
-      <c r="A1" s="7"/>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="A1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="3" spans="6:7">
-      <c r="F3" s="12"/>
-      <c r="G3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="14"/>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="10"/>
-      <c r="D7" s="11" t="s">
+      <c r="A7" s="11"/>
+      <c r="D7" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="7" t="s">
         <v>86</v>
       </c>
       <c r="I7" t="s">
@@ -4690,21 +4722,21 @@
       <c r="N7" t="s">
         <v>91</v>
       </c>
-      <c r="O7" s="6"/>
-      <c r="Q7" s="6"/>
+      <c r="O7" s="7"/>
+      <c r="Q7" s="7"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="10"/>
-      <c r="E8" s="6" t="s">
+      <c r="A8" s="11"/>
+      <c r="E8" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="15" t="s">
         <v>94</v>
       </c>
       <c r="I8" t="s">
@@ -4728,7 +4760,7 @@
       </c>
     </row>
     <row r="9" spans="8:8">
-      <c r="H9" s="15"/>
+      <c r="H9" s="16"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4745,7 +4777,7 @@
   <sheetPr/>
   <dimension ref="D7:N15"/>
   <sheetViews>
-    <sheetView topLeftCell="F4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
@@ -4768,7 +4800,7 @@
   </cols>
   <sheetData>
     <row r="7" spans="4:14">
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="10" t="s">
         <v>98</v>
       </c>
       <c r="E7" t="s">
@@ -5092,32 +5124,32 @@
       <c r="D7" t="s">
         <v>130</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
     </row>
     <row r="8" spans="5:9">
       <c r="E8" t="s">
         <v>133</v>
       </c>
-      <c r="F8" s="6" t="str">
+      <c r="F8" s="7" t="str">
         <f>IAM_ROLE!E9</f>
         <v>role/orgainzation/default/administrator</v>
       </c>
-      <c r="G8" s="6" t="str">
+      <c r="G8" s="7" t="str">
         <f>IAM_LABEL!E10</f>
         <v>organization.gitlab.owner</v>
       </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
     </row>
     <row r="9" spans="5:7">
       <c r="E9" t="s">
@@ -5274,7 +5306,7 @@
   <sheetPr/>
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
@@ -5295,16 +5327,16 @@
   </cols>
   <sheetData>
     <row r="1" ht="18" spans="1:4">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>46</v>
       </c>
     </row>
@@ -5312,62 +5344,62 @@
       <c r="D7" t="s">
         <v>142</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="K7" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="L7" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="M7" s="6" t="s">
+      <c r="M7" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="N7" s="6"/>
+      <c r="N7" s="7"/>
     </row>
     <row r="8" spans="5:14">
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="K8" s="7" t="s">
         <v>150</v>
       </c>
       <c r="L8">
         <f>FD_ORGANIZATION!E8</f>
         <v>0</v>
       </c>
-      <c r="N8" s="6"/>
+      <c r="N8" s="7"/>
     </row>
     <row r="9" spans="5:13">
       <c r="E9" t="s">
@@ -5435,19 +5467,19 @@
       <c r="D7" t="s">
         <v>155</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="7" t="s">
         <v>158</v>
       </c>
       <c r="J7" t="s">
@@ -5538,82 +5570,82 @@
   <sheetPr/>
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.87407407407407" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="3" width="8.5037037037037" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.3777777777778" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.6222222222222" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.6222222222222" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.1259259259259" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22.3777777777778" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21" style="1" customWidth="1"/>
-    <col min="10" max="1025" width="8.5037037037037" style="1" customWidth="1"/>
-    <col min="1026" max="16384" width="8.87407407407407" style="1"/>
+    <col min="1" max="3" width="8.5037037037037" style="2" customWidth="1"/>
+    <col min="4" max="4" width="17.3777777777778" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.6222222222222" style="2" customWidth="1"/>
+    <col min="6" max="6" width="18.6222222222222" style="2" customWidth="1"/>
+    <col min="7" max="7" width="20.1259259259259" style="2" customWidth="1"/>
+    <col min="8" max="8" width="22.3777777777778" style="2" customWidth="1"/>
+    <col min="9" max="9" width="21" style="2" customWidth="1"/>
+    <col min="10" max="1025" width="8.5037037037037" style="2" customWidth="1"/>
+    <col min="1026" max="16384" width="8.87407407407407" style="2"/>
   </cols>
   <sheetData>
     <row r="1" ht="18" spans="1:4">
-      <c r="A1" s="3"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="A1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="7" spans="4:10">
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="J7" s="2"/>
+      <c r="J7" s="3"/>
     </row>
     <row r="8" ht="18" spans="5:10">
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="J8" s="2"/>
+      <c r="J8" s="3"/>
     </row>
     <row r="9" ht="18" spans="5:9">
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="2" t="s">
         <v>170</v>
       </c>
     </row>

</xml_diff>